<commit_message>
The 18th lesson was finished. Onlu Jenkins configuring remain
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="11460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="11460" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId1"/>
+    <sheet name="test_suite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>firstname</t>
   </si>
@@ -45,6 +47,57 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>Raman Arora</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Bim</t>
+  </si>
+  <si>
+    <t>Bam</t>
+  </si>
+  <si>
+    <t>Malkov</t>
+  </si>
+  <si>
+    <t>TCID</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>runmode</t>
   </si>
 </sst>
 </file>
@@ -362,10 +415,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,7 +478,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,8 +491,11 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -400,10 +507,98 @@
       </c>
       <c r="D2" t="s">
         <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>33518</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>33518</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>33518</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>